<commit_message>
Call transcrip sentiment, topic, and summary generated using GPT4o mini
</commit_message>
<xml_diff>
--- a/data/df_10_summary_topic_sentiment_gpt4omini_V2.xlsx
+++ b/data/df_10_summary_topic_sentiment_gpt4omini_V2.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,445 +434,490 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>id</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>processingdate</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>transcription</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>summary_old</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>summary</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>topic</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>sentiment</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>cost</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>18531</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" t="n">
+        <v>18531</v>
+      </c>
+      <c r="D2" t="inlineStr">
         <is>
           <t>2024-09-24 13:44:12</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="E2" t="inlineStr">
         <is>
           <t>Goedemiddag, dit is natuurlijk helemaal Hendrik. Hoi, Sta Bosma van Barbara Bosma. Hallo, hoor je mij? Ik hoor jou. Ja, wij hebben vanochtend een mail gehad van Michaël El Kes. Ja. Over de fooi lamp met flitser. Klopt, ik zie het inderdaad. Ja, ik zit hier samen met met mijn oom dan. De laten we zeggen de technische man. Ja. Wij vroegen ons af want die zo'n flitlamp die hebben wij nog wel, die jullie hebben zeg maar dezelfde soort als dat jullie gestuurd hebben, die hebben we nog liggen van twaalf volt, maar volgens Bram of Michael weet ik nog niet, die zeggen je kan hem zo aansluiten. Wij wij denken dat die gateway er tussen moet, maar want hij moet een signaal krijgen op een gegeven moment. Ja, klopt inderdaad. En ik heb wel eens foto's gestuurd. Er hangt nu al een soort van een zoemer met een ook met een internet aansluiting. Met een IP-adres erop, maar dan daar kan je voor mij niet zomaar die die flits lamp bij je op aansluiten. Want die moeten bijkomen zeg maar. Ja, we hebben nu alleen een zoen, maar we willen ook graag een flits lamp erbij hebben. Die jongens wel eens oordoppen op hebben en dan ze niet. Nee, snap ik. En die flitsland die is zelf geen aansluiting. Ja, die gewoon een plus en een min. Maar kijk maar die die die moet een keer die moet aan die moet aan geschakeld worden als de telefoon gaat natuurlijk. Nee, precies. Ik snap wat je bedoelt. Dus daarvoor denken wij dat wij maar nu staat er in die mail van Bram staat ik zie dat er een netwerk kabel loopt, dus ik denk dat we zo kunnen aansluiten zonder tussenkomst van gateway. Maar dan denk ik ja, waar sluit je hem nog op aan. Goeie, ik zal ik zal even vragen momentje. Ja, dus vanochtend ook nog hierover gemaild. Ja, ik zie het inderdaad hoor, momentje. Ja, maar die die zoomen krijgt ook voeding. Ja. Dat zwarte draadje gaat onder. Die Ik denk ook die keerplaats zie je dat kan nooit. Bedankt voor het wachten. Ja. Ja, dan vermoeden ze dan toch dat er oké beet tussen moet als 'ie alleen een plus en een min heeft. En hij moet Ja, ik weet niet hoe Bram het toen bedacht had. Het enige wat wij denken is dat hij bij die zoemer op moet dan, maar ik weet niet dat kan. Ja, als ik niet echt een eigen netwerk aansluiting heen hoor, dat lastig natuurlijk. Of je niet vanuit de zoemer kunt doorlussen, zeg maar naar Ja, maar bij de De zoemer heeft een IP adres. Ja, hoor je dat? Ja, precies. Die krijgt die krijgt inderdaad bij een inkomen signaal een Ja. We kijken we kunnen straks kijken of daar nog wel een plus of min op zit zeg maar dat we daarbij op aansluiten dan is heel Ja, misschien dat die een output heeft plus min of zo dat zou kunnen. Nou maar dat heeft misschien Bram dan bedacht. Dat denk ik wel ja. Ik denk dat die meer op die manier bedoeld heeft. Ja. Dus waarschijnlijk dat je dan daar gewoon op aangesloten met de plus en de min. Ja en die gateway als je die zouden willen bestellen heb je die zo voor de hand of is dat een speciaal iets of? Ja dat zal eventjes voor je uit moeten. Zo zou ik wel even per mail dan toe moeten sturen. Ja, we moeten even wachten of het vanmiddag lukt. Nou anders scheelt het scheelt jouw werk. Dat maakt niks uit hoor. Nee dat is geen probleem. Dan moet ik dan moet ik inderdaad even uitzoeken of ik die zo voor de hand heb. Je hebt ook die wil veel zo eentje kost. Ja, hij had in een eerdere mail een keer. Ik zeg van het zou rond de honderdtwintig euro kosten voor de fooi K2 of zo. Zie je ze dan zie bijlage k twee. Ik heb een tijdje laten liggen nu moet ik nu gewoon even doorpakken want anders houden jullie er ook even mee bezig en Ik weet niet zo goed die gestuurd heeft hoor. Ik zou ook kunnen hoor. Er zit niks van mij dat wel dat op dat bedrag ligt inderdaad. Dat is op vier november tweeduizend tweeëntwintig geweest. Zo lang loopt het al. Nee, dan moet nou ja, zal ik wel eens terug moeten kijken of die bedacht heeft. Ik zal eens even kijken wat beschikbaar is. Oké, nou ja. Kom ik daarop terug. Best. En wij gaan het proberen om die flitlamp aan te sluiten op die zoomen. Dat dat is eigenlijk het aller makkelijkste als dat zou kunnen. Ja, precies. Voor hetzelfde geld zit er inderdaad een output op vanuit die zoomen. Ja. Dat zal het mooiste zijn. Die zoemer hebben jullie voor mij ooit ook geleverd. Ja, maar dat is wie optie één ga ja. Ja, dat zou ik moeten kijken. Optie één richt zelf inderdaad ook wel wat. Maar dat zou inderdaad kunnen hoor. Die regel niet zoveel veel, vind ik allebei. Oké. Nee dat zou kunnen. Ik weet niet dat moet ik eventjes nagaan dan zeg je als ze dat van ver voor tweeduizend tweeëntwintig loopt dan moet ik even terug zoeken. Ja dat snap ik ja. Oké. Ik kom weer in de lucht als ik er iets gevonden heb. Ja, dank je. Hoi, Astrid. Oké. Hoi, Astrid.</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="F2" t="inlineStr">
         <is>
           <t>Sta Bosma van Barbara Bosma belde met een technische vraag over het aansluiten van een 12-volt flitslamp op een bestaande zoemer. Er is mogelijk een gateway nodig, tenzij de zoemer een geschikte output heeft. Erwin Dijkstra zal nagaan of de gateway beschikbaar is en wat de kosten zijn, en zal hierover per e-mail terugkomen. Sta zal in de tussentijd proberen de flitslamp direct op de zoemer aan te sluiten.</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="G2" t="inlineStr">
         <is>
           <t>Hendrik heeft gesproken met Sta Bosma over de aansluiting van een flitslamp op een zoemer. Er werd besproken dat de flitslamp een signaal nodig heeft en dat er mogelijk een gateway tussen moet. Hendrik zal uitzoeken of de benodigde gateway beschikbaar is en komt hierop terug. Sta Bosma en zijn oom zullen proberen de flitslamp aan te sluiten op de zoemer.</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="H2" t="inlineStr">
         <is>
           <t>technische ondersteuning flitslamp</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="I2" t="inlineStr">
         <is>
           <t>neutraal</t>
         </is>
       </c>
-      <c r="H2" t="n">
+      <c r="J2" t="n">
         <v>0.000644</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>18526</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" t="n">
+        <v>18526</v>
+      </c>
+      <c r="D3" t="inlineStr">
         <is>
           <t>2024-09-24 13:18:10</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="E3" t="inlineStr">
         <is>
           <t>Goedemiddag, Michel. Hey, Michael met Carla VW elektro service. Hallo. Ben jij op de hoogte van een storing bij ons? Nee. Nee? Heb ik? Nee. Nou, ik krijg in mijn telefoon en ik bel nu met mijn eigen mobiel dan hoor, maar registratie bij provider mislukt. Ik zie ook inderdaad dat de giga set ook offline is. Ja. Is er iets bekend bij de internet provider of stroomstoring? Ik heb net nou stroomstoornissen, want dat werkt allemaal. Maar ik heb bij Ziggo eventjes gekeken online of de storing in deze regio is, maar dan geeft hij niks aan inderdaad. Oké. En je hebt verder op de computer of voor laptop heb je wel internet. Nou, ga nog eens even kijken boven of die doet. Maar ik had inderdaad jullie doorgeschakeld naar mijn collega, dus mijn collega krijgt jullie de telefoon. Ja. Als dat wel werkt. Maar die kreeg ik ook niet de geschakel, kinderen. Even kijken hoor. Ik zat beneden. Ja, dat klopt inderdaad. En jullie bellen naar een schakelaar aan, maar op het moment dat de hand zet offline is Dan kun je hem naar stories inzetten alleen zie je ook dat die nou nu bij Joan binnenkomt. Ja, ja, ja dat weten ze hoor. Dus dat klopt, ja. Ja, dat is goed. Even kijken of ik nou wel internet heb. Dat hij het wel of niet doet. Nou ik denk inderdaad dat ook de internet het niet doet. Nee, nee, hij doet het niet. Nee. En de je had zich al verder niet gesproken, je had zelf even gecheckt. Ja, ik heb even online gecheckt. Ik weet niet of je of je weet waar het modem zit. Wellicht die een keer een huishoud geven, wat dat voldoende is. Maar als je dat niet aandurft dan zou ik even contact met Ziggo. Ga ik even doen. Ik weet wel iets hoor, maar ik ga zich wel even bellen. Ja, helemaal goed. Dank je wel in ieder geval weer. Ja, helemaal goed, graag gedaan. Dank je. Hoi.</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="F3" t="inlineStr">
         <is>
           <t>Carla van VW Elektro Service belde Michael Kes over een storing waarbij de registratie bij de provider mislukt, resulterend in geen internetverbinding en een offline Gigaset. Carla heeft gecontroleerd op storingen bij Ziggo, maar er zijn geen meldingen. Michael adviseerde om het modem te resetten of contact op te nemen met Ziggo voor verdere hulp. Carla gaat contact opnemen met Ziggo.</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="G3" t="inlineStr">
         <is>
           <t>Michael van 10Telecom heeft gesproken met Carla van VW elektro service over een storing bij hun internetverbinding. Carla meldde dat de registratie bij de provider mislukt en dat de giga set offline is. Michael heeft geadviseerd om het modem te controleren en eventueel contact op te nemen met Ziggo voor verdere ondersteuning.</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="H3" t="inlineStr">
         <is>
           <t>storing internetverbinding</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
+      <c r="I3" t="inlineStr">
         <is>
           <t>neutraal</t>
         </is>
       </c>
-      <c r="H3" t="n">
+      <c r="J3" t="n">
         <v>0.000387</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>18522</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="n">
+        <v>2</v>
+      </c>
+      <c r="C4" t="n">
+        <v>18522</v>
+      </c>
+      <c r="D4" t="inlineStr">
         <is>
           <t>2024-09-24 13:08:11</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="E4" t="inlineStr">
         <is>
           <t>Hitler van Mikoell. Hallo, Miko. Goed. Mijn naam is Olivia en ik kom link van Akstal, die manufacture of die ICT Correct. Oké, perfect. Zelfs jullie have al dit is. Dank je wel, Maud voor voor de informatie en hij wil twee te doen is dat correct het personeel aan de erbij. Nou probleem. Je was. Thanks, heb een good ding. Bye, bye. Thanks, bye.</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="F4" t="inlineStr">
         <is>
           <t>Olivia van Akstal heeft contact opgenomen om informatie te verstrekken over een ICT-manufacture. Ze bevestigde dat alle benodigde informatie al beschikbaar is en bedankte Maud voor de hulp. Er zijn geen verdere acties of problemen gemeld.</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="G4" t="inlineStr">
         <is>
           <t>Olivia van Akstal belt om informatie te bevestigen over ICT en personeel. Er zijn geen specifieke oplossingen of vervolgacties besproken.</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="H4" t="inlineStr">
         <is>
           <t>ICT en personeel</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr">
+      <c r="I4" t="inlineStr">
         <is>
           <t>neutraal</t>
         </is>
       </c>
-      <c r="H4" t="n">
+      <c r="J4" t="n">
         <v>0.000227</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>18509</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="n">
+        <v>3</v>
+      </c>
+      <c r="C5" t="n">
+        <v>18509</v>
+      </c>
+      <c r="D5" t="inlineStr">
         <is>
           <t>2024-09-24 11:54:31</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="E5" t="inlineStr">
         <is>
           <t>Met Peter Fritswijk. Dag Peter met Gerwinant, team telecom. Goeiemorgen. Hi Gerwinant. Hi hallo. Mooi mooi. Een drukke ochtend. Ja, We hebben elkaar even te pakken. Ja, super super. Hey ik ik ik ik ik klopt dat je dat je woont in Duitsland? Ja, ik woon in Natland. Ja, oké nou dat is vlakbij ons zeg maar, wat dat er gaat. Ja, nou ja, ik kom zelf op de Oldezaal dus Ja, precies oké. Een Duitse vrouw die ik ken, ja. Ja, ja. Mijn neef die woont zelf ook in Duitsland die woont in in Coevorden zeg maar in Laren heet dat volgens mij. Ja, ja, ja. Daar kon ik regelmatig. Ja, nee. Vrienden wonen dus. Oké, dat is mijn neef Dinand zeg maar die heeft ook een bedrijf in Hardenberg, een tekst een tekstbureau zeg maar. En dat heeft hij na een aantal jaren al inmiddels. Mensen ook wat meer inzicht krijgen in in de techniek waar wij dan in zitten. Dat men daar een beeld bij is zeg maar. Ja, precies ja, nou ik ken het principe dus ik ben niet bekend met contact en alles al. Nee, ik ben wel geweest op je website alleen ik ben er niet mee bekend. Nee, dus ongeveer hetzelfde wat jij doet dus echt de communicatie voor bedrijven en ik laat wel even wat we daarbij doen dan. Oké, Ja, want ik ik Even kijken, Johan is het bedrijf in Nederland. En ik zal ik dan denk ik op de op de verkeerde als je het training Ja, nee, Saycon is ons naam. Ik heb nu veel contact. Dat is een soortgelijk bedrijf wat jij hebt in Oldenzaal. Ja. Dus die zit voornamelijk ook in Twente land en in de Achterhoek. Ja, oké op die manier. Ja. Want jullie hebben meerdere bedrijven begrijp ik. Nou, wij hebben wij hebben zelf drie bedrijven, vier bedrijven. Cirkel is onze handelsnaam handelsnaam. Ja. Qip Work dat is een uitzendbureau onder zitten. Qip pay bedrijf. Qip HRM en dat is echt HR vaak en salaris verwerking. Ja. En dan hebben we intermens oude dienst die we daarnaast hebben. Ja, oké op die manier. Volledig h r dienstverlening. Ja en bij welk bedrijf ben jij dan werkzaam? Ik zit ja, ik val onder de cirkel. Dus gewoon onder de groep, maar ik werk voornamelijk voor de payroll kant en de hele kant. Ik ben eind verantwoordelijk voor alle gedetacheerde uitzendkrachten en pay rollers. Ja, oké. Oké en je doet het vanuit waar is het kantoor dan bij jullie? In Hengelo. Hengelo oké op die manier, ja. Oké ja, ik ben begonnen zeg maar met tien telecom en achternaam is boer tien dus daar komt tien telecom vandaan. Begon in tweeduizend vijf en toen was vibe telefonie nog redelijk onbekend zeg maar dat doen ze opmars wel, maar in die periode behoorlijke stappen kunnen maken zeg maar wat uiteindelijk dat we uitgegroeid zijn tot een zelfstandige provider, dus wij zijn aangesloten bij vereniging Coin. We hebben onze eigen Coin code, want Nederland telt zeg maar iets van honderdvijftig providers een KPN, een Foreovoo, maar ook aan het spelen team Telecom. Ik ben toen in tweeduizend zeven ben ik samen gaan werken met de Jacob Jacob die hadden een bedrijf Senosite die verkochten de internetverbinding in Nederland en samen met hun de voIP kant opgepakt zeg maar en dat zijn behoorlijk wat klanten die hadden interesse toen ook al in voIP en die hebben wij dus kunnen aansluiten. Ja, en vervolgens hadden wij ook een telefooncentrale waarmee werkte dus zoiets als Helion zeg maar, alleen het was wel een ander merk en ja, we hebben in de afgelopen jaren hebben we wat overnames gedaan van telecom bedrijven hadden we iets van vijf verschillende telefoonscentrales in beheer. Dat is niet te doen want ja het is software en iedere software heeft zijn eigenaardigheden. Dus van daaruit zijn we met een buitenlandse software ontwikkeld bedrijven in contact gekomen want heel veel systemen zeg maar voor bijvoorbeeld is op Astraest gebaseerd. Ik weet niet of je dat niet zegt. Nee dat zegt niet zoveel. Nee oké. Het is wat dat dan gaat is heel veel systemen zijn zeg maar op Astraest gebaseerd en daar hebben we onze eigen platformen en dat noemen we dan pring. Pring punt nu is dan de website daarvan en dat ons platform die wordt gebruikt bij ons. Maar we werken daar nu ook samen met resellers, we hebben iets van zeventig resellers zitten in heel Nederland die dus onze producten dus ook adviseren bij hun klanten. En ja, dat in afgelopen jaren gaan doen en ja, een mooie stabiele stabiel bedrijf neer kunnen zetten. En ja en nu volop in ontwikkeling met AI dus die meeting die ik net had zeg maar. Dat we hebben nu een deel gaan we out uitbesteden en daar moet je bijvoorbeeld aan denken bedrijven die gesprekken voeren dan maken wij van het gesprek maken wij een transcriptie en vervolgens van die transcriptie maken wij daarvan een samenvatting en daar halen we de hoogtepunten uit want veel bedrijven zeg maar die maken altijd van een gesprek een gespreksverslag, zodat je na die tijd altijd goed beslagen ineens weer komt bij degene die hebt gesproken lees die even in kun je zo'n samenvatting lezen. Ja en dat geeft op dat moment een goed inzicht van het gesprek zeg maar. Alleen we willen daar een stapje in verder gaan dus dat je bijvoorbeeld een manager bijvoorbeeld kan zeggen van nou ja waar afgelopen week hoeveel gesprekken zijn er geweest 10 opzichte van de week ervoor. Nou daar komt dan een resultaat uit kun je aangeven waar het meeste wordt voor gebeld. Nou ja, weet je het GPT-achtige vragen kun je dan stellen zeg maar en daar daar hebben we net een stap meegemaakt dat we daar verder in gaan verdiepen zeg maar. Is interessant. Ja, dus wat dat betreft, ja, het is een ja, een Voite telefonie dus bellen via internet zeg maar, ja, dit is afgelopen jaren is dat behoorlijk veranderd en ja, de manier van bellen is ook ja, vroeger had je altijd een toestel op je bureau staan en tegenwoordig is het heel normaal dat je belt via je computer of via Microsoft Teams is ook een optie of misschien wil je toch nog steeds het toestel hebben staan op je bureau. Dus en van daaruit ja, die ontwikkelingen die waren er al en ja daar komt in één keer AI om doen kijken. Dus ook als je bijvoorbeeld belt naar ons we hebben een AI gestuurde keuzemenu dus als je zegt van joh ik heb een aanmaning ontvangen ik heb daar een vraag over dan weet die dat die de callflow in moet voor administratie, maar heb je een ja, ik ben een hr vraag bijvoorbeeld, ja dan zou die zich ook bijvoorbeeld dat die dat kwalificeert en dat je dus die naar richting de hr afdeling kan sturen bijvoorbeeld. En daar daar zijn we dan mee bezig zeg maar bij ons. Ja, maar dat is Cat en we zijn, we hebben nu een serie om waar we mee werken. Ja. Voor zeker is het voor ze het ideaal omdat we ja, veertig procent werken of vanuit huis. Ja. Dus dan is het gewoon op de app heel makkelijk op inloggen en je kan gewoon bellen. Precies, ja. Maar ja, ik ben daar niet zo heel tevreden over. Ik Ik ben in het verleden ben ik en ze zullen ongetwijfeld afgelopen jaren behoorlijk doorgegroeid zijn zeg maar dat het systeem is natuurlijk veranderd. Maar ik ken ze vanuit het verleden en toen wat ik net al aangaf ik had toen in eerste kant had ik een centrale die ik kan teren ik wilde daarnaast ook een ander alternatief hebben toen ben ik mij ook gaan verdiepen in Céon. Ik ben zelfs pater geweest van hun. Echt nooit nooit een een saden van hun aan kunnen sluiten bij een klant niet en puur om het feit dat met het systeem wat ik al laat zeg maar die kon ik was breder inzetbaar dan Seelion. Seelion was net even ja dat was niet niet het product waar ik graag mee samenwerkte. Dus naar en eigenlijk in de afgelopen jaren zeg maar hebben we dus die vijf telefooncentrales alle goede dingen daarvan hebben dus nu gestopt in onze eigen telefooncentrale train. Ja, en daar daar maken we nu bedrijven mee bereikbaar zeg maar en ik ja, als je dan ziet wat voor mogelijkheden je dan hebt dat dat laat heel goed met zich koppelen bijvoorbeeld met een CRM ERP systemen maar ook bijvoorbeeld die AI diensten die we dus nu ook bieden. Ik zit aan het MT van bedrijf. Ik moest me even een beetje gaan verdiepen hierin. Dus jij Alsof je wist dat je mij moest benaderen. Ja, nou ik moet zeggen wij wij zijn ook sinds een half jaar terug denk ik gaan samen met een marketing bedrijf, zelfde verhaal die kwam ook bij mij binnen en ook op het juiste moment we waren net op zoek toen naar iemand anders want we deden zaken met bedrijven in Deventer. Nou ja, we komen met hun om tafel en het is gewoon een goede klik tussen ons en ja, dat is dan het moet zo lopen zeg maar soms. Ja. Heb jij documentatie hierover? Ik heb geen folder of brochure, ik kan je daarover wel een email sturen met even wat informatie van de producten en diensten die we bieden. Ja. Dus dat is ja, dat heb ik wel, zeker. Ja, nee, maar dan kan ik, we hebben maandag m t overleg. Ja. Dus ook eventjes kijken en de afgelopen week hebben we het erover gehad, dat ik me daar zo gaan verdiepen. Want jullie wel jullie willen erg wat anders dan. Wij willen iets, we hebben altijd een telefoniste gehad. Ja. Daar zijn we mee gestopt. We willen eigenlijk meer naar één centrale die gewoon op ja, op woord kennen zegt van oké die moet daar naartoe, die moet daar naartoe. Ja, precies, ja, ja. Daarin ook dat ze het gekoppeld is met ons CRM systeem super overigens dat de inkomen telefoontje ook gelijk geregistreerd worden zodat we weten wat er gebeurt Ja, precies precies. Ik maak even gelijk wat notities. Ik denk dat je een e-mailadres hebt waarop je bereikbaar bent. Ja, dat is p punt freeswijk. Ja. Met cirkel punt n l. Cirkel is met een q. Cirkel ja ja ja. CIRQ0N. Ja, punt n l. Staat ook op jouw profiel volgens mij heel duidelijk. Punt n l zeg je? Ja. Oké en wat zijn nog eventueel dingen waar je nu nog meer tegenaan loopt, want het geldt dan voor jullie vier bedrijven? Ja, dat geldt voor alle bedrijven. We werken allemaal met hetzelfde systeem. Maar ook ja, kijk in het arbeidsmarkt. Ja. Zijn we eigenlijk vanaf maart actief meer de markt opgegaan. We merken dat wij wij willen onze zes nummers eigenlijk niet prijs geven, maar ik heb mijn zus overal al staan. Ja. Dat twintig jaar een arbeidsmiddel bemiddeling. Ja. Mijn nummer is overal bekend, dus ja, dus die hou ik gewoon. Ja. Maar ja, wij vinden het lastig mijn collega's die hebben gezegd wij willen ons privé mobiel niet gebruiken. Nee joh. Maar we missen een WhatsApp functie, omdat gewoon bij sollicitanten dat het veel WhatsApp veel makkelijker gaat. Ja. Dat is natuurlijk iets waar wij naar aan het kijken zijn of zoiets ook te integreren is. Ja, nou bijvoorbeeld wij hebben dan op onze website hebben we de mogelijkheid om te chatten zeg maar met ons en daar is dan gekoppeld aan WhatsApp business. Wat vervolgens als iemand chat met ons dan dan pakt een collega pakt dat op bij ons en vervolgens kun je chatten met elkaar. Ja. Ja, kijken we wel even naar of het iets is waar het ook voor ons passend is, maar ik ben wel zeer geïnteresseerd om eventjes met te verdiepen in jullie bedrijf. Ja, nou ja, ik ik ik zal het zo goed mogelijk proberen even uit te leggen in de mail straks zeg maar, Jullie werken veel vanuit huis zeg je? Ja. Oké, en jullie nog heb je nu nu al iets dat je zegt van ja, wat we nu hebben dit werkt gewoon heel fijn en daar willen we zo blijven houden? Ja, het uitbellen gewoon. Eigenlijk het standaard bellen dat moet gewoon blijven dat iedereen wel zijn eigen rechtstreekse nummer in qua mensen uitbellen. Ja, ja, want jullie keuze kunnen hebben, dus stel je voor dat ik dat de collega op vakantie is. Dat ik dan als ik een antwoord dat ik de telefoon opneem, dat er een centrale nummer standaard erin komt en niet mijn nummer die ik waarmee ik opneem. Nee precies, nee want juist Dus als ik opneem dan komt mijn nummer bij in beeld. Terwijl misschien niet eens voor mij bedoeld is, maar omdat ik een telefoon heb genomen met het kreeg in die jas. Nee, oké, op die manier. Je kunt op het telefooncentrale zeg maar kun je zelf bepalen welk afzetnummer je meestuurt. Wil je dat van bedrijf één, twee, drie of vier hebben? Dat kan. Maar heeft een afdeling ook bijvoorbeeld een eigen nummer. Dan kun je ook een afdelingsnummer meesturen. Ja. Dus dat soort zaken zeg maar, maar dat is gewoon eigenlijk een standaard iets wat wat gewoon erbij in zit inderdaad. Die transcripties die kan bijvoorbeeld wat ik net ook al aangaf dat kan dat kan jullie gewoon heel veel inzicht geven. Ja, ik bedoel in gesprek als je tijdens een gesprek die voert constant mee moet schrijven kost krijg je misschien niet alles voor mee heb je niet goed alles genoteerd. Nou in die transcript is gewoon hoe dan ook het hele gesprek wordt voor trends Cloud naar tekst en daar haalt hij zijn samenvatting uit en dat is dan één gesprek en zo wil ik dan straks in de toekomst het mogelijk maken dat dan men daar vaak over kan stellen van een compagnon bijvoorbeeld van mij, René wat ik het al aangaf, die heeft ook een bedrijf in energie. Nou die die Alle gesprekken worden daar opgenomen. Maakt ze daar prijsafspraken of wanneer die teruggeboekt wordt omdat je teveel taal hebt. Dat wordt heel netjes omgezet. Dat haal je eruit zeg maar. Ja, en de manier van bellen want binnen Caleon Ik bel je dan op dat moment ook alweer? Want dat gaat ook via de computer toch? Ja, via de computer. Ja. En dan bel ik altijd ik ben altijd standaard uit met mijn eigen vaste nummer van Cirkel. Ja, precies. Als ik opneem dan krijgt de bellet mijn nummer te zien. Terwijl ik daar zitten alle belds. Jelle krijgt jouw nummer te zien, dus jouw rechtstreekse nummer waarop je bruikbaar bent in plaats van het centrale nummer. Dus als je naar het centrale nummer belt en ik neem op, ik zie automatisch dat ik het heb ben en met mijn nummer. Ja, oké, ja, oké, ja dat kan, ja. Ja, en ja, ik weet niet of jullie daar behoefte aan hebben, maar je kunt dus bij ons ook bellen via de computer, dus dan lach je gewoon in en ben je daarop bereikbaar. Maar heb je de computer uitstaan, dan zouden we ook eventueel gebruik kun je maken van onze app die je installeert op je smartphone. Precies. Ik doe altijd via mijn mobiel uit. Ja, oké. Nou dat is bij ons ook het geval en op dat moment als je computer uit hebt staan dan ben je daar alsnog op bereikbaar of eventueel in de auto. Dus stel Jet, toestelnummer, ik noem het alle alle telefoonscentrales werken met een intern nummer. Dus bijvoorbeeld toestel tweehonderd één kunnen we laten rinkelen op de computer, maar ook op je smartphone bijvoorbeeld. Mocht je onderweg zijn dus op die manier kunnen wij dat inrichten inderdaad. Nou ja en en die interactieve keuzemenu zeg maar dat dat kun je dus ook bij ons gebruik van maken dus als bijvoorbeeld zou bellen naar Rand en je zoon zeggen van ik ben op zoek naar Gebrand en dan komt die bij mij uit zeg maar. Nou wat ik al zei Ik ik wil een uitzendkracht dan komt hij ook bij arbeidsmarkt terecht terecht. Precies, juist correct. Op die manier kan een hand versterkt worden herkent die dat en zet die niet door en en mocht er ja zeg maar iets niet herkend worden dan kan die alsnog bijvoorbeeld naar een groepje overige waar dan aantal medewerkers zitten die dus die niet gecategoriseerd kan worden dat hij alsnog binnenkomt zeg maar. Ja, nou duidelijk. Ja, ik ga even wat informatie bij elkaar verzamelen en dan stuur ik het naar je toe. Mocht dat jullie wat lijkt of wat dan ook. Ik kom ook met alle plezier en kennen jullie toe om wat dingen te laten zien hoe het systeem werkt en wat het kan en doet zeg maar. Dus dat kan ook. Goed om te horen. Wat ik aangeeft maandag hebben we even een MT overlegd, dat is het eind van de dag. Ja. Dus vanuit dinsdag en half vannacht dan even contact met je opnemen. Ja, dat is goed. Nee, want als ik even mag kijken nagaan hoeveel gebruikers heb je het ongeveer over dan waar we nu Wij zitten nu met tweeëntwintig medewerkers. Ja, oké. En dat is op één vestiging? Is op twee vestigingen. Ja, oké top. Nou ik ga wat uitwerken en ja, ik laat je wat zien en ik mocht het niet duidelijk zijn of wat dan ook laat het ook gerust weten dan, dan ga zeggen. Oké, nou bedankt voor je belletje. Ja, is goed jij ook bedankt interesse en dan hebben we nog even weer contact. Oké, doei doei.</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="F5" t="inlineStr">
         <is>
           <t>Gerwinant van 10Telecom had een gesprek met Peter Fritswijk over de geschiedenis en diensten van 10Telecom, waaronder hun focus op VoIP-telefonie en het gebruik van AI voor gespreksanalyse. Peter toonde interesse in een spraakherkenningscentrale gekoppeld aan hun CRM-systeem en een oplossing voor het gebruik van WhatsApp zonder privé mobiele nummers. Hij vroeg om documentatie en verdere informatie over de producten en diensten van 10Telecom. Zijn e-mailadres is p.freeswijk@cirqon.nl.
 Daarnaast belde een klant om te bespreken hoe 10Telecom hun telefoniesysteem kan verbeteren voor thuiswerken. Ze willen dat medewerkers hun eigen rechtstreekse nummer behouden bij uitgaande oproepen, maar dat bij het opnemen van oproepen een centraal nummer wordt weergegeven. Ze bespraken ook de mogelijkheid om gesprekken via de computer of een app op de smartphone te voeren en het gebruik van interactieve keuzemenu's. De klant heeft 22 medewerkers verdeeld over twee vestigingen en zal na een MT-overleg op maandag dinsdag contact opnemen voor verdere bespreking.</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
+      <c r="G5" t="inlineStr">
         <is>
           <t>Gerbrand Boertien heeft een gesprek gehad met Peter Fritswijk over telecomdiensten en de mogelijkheden van samenwerking. Peter is geïnteresseerd in de producten en diensten van 10Telecom, vooral in verband met hun behoefte aan een centrale telefonieoplossing die geïntegreerd kan worden met hun CRM-systeem. Gerbrand zal Peter een e-mail sturen met meer informatie over de producten en diensten, en Peter zal na hun MT-overleg contact opnemen om verdere stappen te bespreken.</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr">
+      <c r="H5" t="inlineStr">
         <is>
           <t>telecomdiensten en samenwerking</t>
         </is>
       </c>
-      <c r="G5" t="inlineStr">
+      <c r="I5" t="inlineStr">
         <is>
           <t>positief</t>
         </is>
       </c>
-      <c r="H5" t="n">
+      <c r="J5" t="n">
         <v>0.001493</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>18498</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="n">
+        <v>4</v>
+      </c>
+      <c r="C6" t="n">
+        <v>18498</v>
+      </c>
+      <c r="D6" t="inlineStr">
         <is>
           <t>2024-09-24 11:24:16</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="E6" t="inlineStr">
         <is>
           <t>Ik vind het wel mooi van. Dag, goedendag. Met Richard van de Zwalspetje. Ik vroeg naar Eric. Ik ga voor je tijd. Hij was toevallig met je mail bezig. Moment. Oké. Graag voor het wachten, Hendrik. Dag Hendrik Richard van de zaal spreek je weer. Hoi. Ik ben nu niet blij en ik heb geen internet dus dat is een heel vervelend natuurlijk want dan heb ik een dure bundel. Ik heb gister echt in de stress gezeten twee uur je ronde bezoek gehad. Ja. En ik hoop dat die zijn rekening bij jou gaat deponeren niet bij mij want ja nogmaals dat is allemaal niet ik heb een abonnement bij jullie dat gewoon iets functioneerde dat had dan open gezet hoop ellende en nu ben ik op op zestien nou Rotterdam Airport. Kan bel bellen, kan nu wel gebeld worden. Ik heb een berichtje gekeken naar YouFon gegaan, maar ik heb geen internet. Heb je toestel ook een herstart al gegeven? Wat zeg je? Heb je toestel ook al een herstart gegeven? Nee, nog niet. Want ik was net bezig met jouw mail, want het kan wel gewoon komen omdat de eSIM geïnstalleerd geactiveerd was voordat de koppeling daar werkt was verwerkt. Oké. Want de instellingen zowel binnen Nederland als in de EU met betrekking tot data en voice staan gewoon allemaal goed. Ook de data zou moeten werken, maar ik denk omdat het komt dat ISMA voordat de potering is verwerkt geactiveerd is. Ga ik hem even aanzit en uitzetten en dan hoop ik dat hij het doet en laat ik het nog even weten. Ja, is goed is goed. Dan bel mij eventjes op.</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
+      <c r="F6" t="inlineStr">
         <is>
           <t>Richard van de Zwalspetje belde met Hendrik Stuiver over een internetstoring, wat voor veel stress zorgt. Hendrik suggereerde om het toestel te herstarten vanwege een mogelijke eSIM-issue. Richard zal dit doen en Hendrik op de hoogte houden van de resultaten.</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
+      <c r="G6" t="inlineStr">
         <is>
           <t>Richard van de Zwalspetje belt omdat hij geen internetverbinding heeft, ondanks zijn dure bundel. Hendrik Stuiver legt uit dat de eSIM mogelijk te vroeg is geactiveerd voordat de koppeling was verwerkt. Hendrik adviseert Richard om zijn toestel opnieuw op te starten en vraagt hem om terug te bellen met een update.</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr">
+      <c r="H6" t="inlineStr">
         <is>
           <t>internetproblemen</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr">
+      <c r="I6" t="inlineStr">
         <is>
           <t>ontevreden</t>
         </is>
       </c>
-      <c r="H6" t="n">
+      <c r="J6" t="n">
         <v>0.000363</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>18497</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="n">
+        <v>5</v>
+      </c>
+      <c r="C7" t="n">
+        <v>18497</v>
+      </c>
+      <c r="D7" t="inlineStr">
         <is>
           <t>2024-09-24 11:23:09</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="E7" t="inlineStr">
         <is>
           <t>Hoi, mooi. Nou daar ben je hem hoor. Ja, is goed ja. Komt 'ie. Volgens mij snapte 'ie ook niet dat ik hem geen dol voor binnen. Oké.</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
+      <c r="F7" t="inlineStr">
         <is>
           <t>Er is geen samenvatting mogelijk omdat de oproep geen duidelijke informatie bevatte over de reden van het gesprek, de besproken oplossingen of eventuele vervolgacties.</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
+      <c r="G7" t="inlineStr">
         <is>
           <t>De 10Telecom collega sprak met de klant over een misverstand. De klant leek niet te begrijpen dat er geen dol voor binnen was. Er zijn geen specifieke oplossingen of vervolgacties besproken.</t>
         </is>
       </c>
-      <c r="F7" t="inlineStr">
+      <c r="H7" t="inlineStr">
         <is>
           <t>onduidelijkheid</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr">
+      <c r="I7" t="inlineStr">
         <is>
           <t>neutraal</t>
         </is>
       </c>
-      <c r="H7" t="n">
+      <c r="J7" t="n">
         <v>0.000228</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>18496</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="n">
+        <v>6</v>
+      </c>
+      <c r="C8" t="n">
+        <v>18496</v>
+      </c>
+      <c r="D8" t="inlineStr">
         <is>
           <t>2024-09-24 11:16:14</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
+      <c r="E8" t="inlineStr">
         <is>
           <t>Goedemorgen, jullie komen Hendrik. Ja, goedemorgen met Elleichgelaar van het samenwerkingsverband Zuid Oost-Friesland uit Drachten. Hallo. Hallo, ik heb even een vraagje. Ik heb wat nieuwe collega's gekregen en ik moet die telefoon hebben ze invoeren via een Euro Euro van jullie, sorry hoor. En Ja. Maar ik heb niet meer dat linkje. Want dat is al heel lang geleden dat ik dat gedaan heb. En ik weet eigenlijk niet meer hoe ik daarin moet komen. Kunt u mij daaraan helpen? Even kijken. En het kan ook wel via de telefoon, maar ik ik weet dat ik dat ik moet ook mensen eruit halen. En ik denk dat vind ik toch fijner om dat even te doen, maar ik doe dat haast nooit. En dan weet ik niet meer hoe ik dat moet doen zeg maar. Ik heb wel een briefje ooit van jullie gekregen met een lamp. Ja, maar dan wordt ze worden door gegaan naar nul zes nummer zie ik. Ik zie het hoofd nummer bijvoorbeeld en dan ja, dan hebben ze daar centrale en twee nul één gebruiker. Ja, klopt inderdaad. Maar die ja, we gebruiken als helemaal die vaste toestellen nou allemaal niet meer. Oké. Maar ik moet gewoon even wat nul zes nummers in de in de lijst zetten. Maar dan kon ik altijd via een via jullie website ergens invullen, zeg maar. Klopt, ik zal ik even En als ik even zo'n linkje kan krijgen hoe daarin komt, snap je? Zeker. Of kan dat niet? Jazeker zeker. Rustig. Op welk mailadres had jij een account? Op info at Ja. SWVZ0 Friesland punt NLS Simon Duric Zagaas Victor Otto. S Simon Willem Victor Zagaas Otho. Ik zie het hè. Een w van Willem is het. Ja, nee, excuus. Heb je het wachtwoord nog wel? Nou, dat is al heel oud. Oké. Want ik ik heb het op een briefje hier in Malaar liggen, maar was zo lang geleden dus. Er staat wel een een wachtwoord op van zes CVFFFMN that zoiets is wat het. Ja, ik ik stuur anders wel een nieuw wachtwoord en in die mail staat ook gelijk waar je kunt inloggen. Fijn. Dan hebben we gewoon alles in één kant klap. Ja, mooi. Zo. Info at Nou, ontvang van mij zo een mailtje met daarin een een link en daar staat dan klik je hier. Ja. Als je daarop klikt dan kom je op een website terecht een beveiligde link die eenmalig te openen is. Ja. En dan krijg je ook een optie te zien view notes. Als je daarop klikt dan zie je het wachtwoord. Oké, view notes. Hartstikke fijn, mooi zo. Nou dan kom ik er vast wel uit. Alvast wel, zeker weten. Anders bel me eventjes op hoor. Ja, helemaal goed. Mooi zo. Oké. Bedankt. Doeg. Doeg. Doeg.</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
+      <c r="F8" t="inlineStr">
         <is>
           <t>Elleichgelaar van het samenwerkingsverband Zuid Oost-Friesland uit Drachten belde met Hendrik Stuiver omdat hij nieuwe collega's moet invoeren in het telefoonsysteem van 10Telecom, maar hij is de inloglink kwijt. Hendrik stuurt een nieuwe inloglink en een nieuw wachtwoord naar het opgegeven e-mailadres (info@swvz0friesland.nl). Elleichgelaar kan via deze link inloggen en de benodigde wijzigingen doorvoeren. Hendrik gaf aan dat Elleichgelaar kan terugbellen als er verdere hulp nodig is.</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
+      <c r="G8" t="inlineStr">
         <is>
           <t>De klant, Elleichgelaar van het samenwerkingsverband Zuid Oost-Friesland, vroeg om hulp bij het inloggen op de website van 10Telecom om nieuwe collega's toe te voegen en oude nummers te verwijderen. Hendrik Stuiver bood aan om een nieuw wachtwoord te sturen naar het opgegeven e-mailadres, inclusief een link voor inloggen. De klant was tevreden met deze oplossing en gaf aan dat hij contact zou opnemen als er verdere problemen waren.</t>
         </is>
       </c>
-      <c r="F8" t="inlineStr">
+      <c r="H8" t="inlineStr">
         <is>
           <t>ondersteuning bij inloggen</t>
         </is>
       </c>
-      <c r="G8" t="inlineStr">
+      <c r="I8" t="inlineStr">
         <is>
           <t>positief</t>
         </is>
       </c>
-      <c r="H8" t="n">
+      <c r="J8" t="n">
         <v>0.000485</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>18492</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="n">
+        <v>7</v>
+      </c>
+      <c r="C9" t="n">
+        <v>18492</v>
+      </c>
+      <c r="D9" t="inlineStr">
         <is>
           <t>2024-09-24 11:08:21</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="E9" t="inlineStr">
         <is>
           <t>Hendrik. Hi, goeiedag met Ersselique van mTL. Hoi. Hoi, ik heb net zo'n vraagje. Ik kreeg een mailtje dat wij bijna door onze bundel zijn, we hebben drie keer vijfhonderd minuten. Klopt. En wanneer tot wanneer loopt dat? Is dat tot rekenen jullie altijd tot het begin van de maand of hoe? Van de eerste tot de laatste dag van de maand geldt de bundels en Ja. Nieuwe bundel, wat een nieuwe bundel weer ja, wat er weer een nieuwe bundel actief drie keer vijfhonderd zo wat is en Ja, dat is maand volgende week dinsdag dan oké. Ja, nee dan dan is dit wel voldoende denk ik. Zo niet ja, gaan we er ietsjes overheen. Klopt ja, nou ja, dan betaal je standaard tarief. Ja. Ja, als dat eenmalig is dan valt het wel mee. Ja of kan gewoon Nee klopt. Nee dat is ook, maar goed voor nu denk ik dat het oké is en Oké. Oké, dank je wel. Alsjeblieft. Hey, hoi. Fijne dag hoi. Zo</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
+      <c r="F9" t="inlineStr">
         <is>
           <t>Klant Ersselique van mTL vroeg naar de vernieuwing van de bundel van drie keer vijfhonderd minuten. Hendrik bevestigde dat de bundel van de eerste tot de laatste dag van de maand geldt en dat er volgende week dinsdag een nieuwe bundel actief wordt. Ersselique was tevreden met deze informatie en gaf aan dat er mogelijk iets over de bundel heen gegaan wordt, maar dat dit geen probleem is. Geen verdere acties nodig.</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr">
+      <c r="G9" t="inlineStr">
         <is>
           <t>De klant, Ersselique van mTL, vroeg naar de status van hun belbundel van drie keer vijfhonderd minuten en wanneer deze verloopt. Hendrik bevestigde dat de bundel loopt van de eerste tot de laatste dag van de maand en dat de nieuwe bundel volgende week dinsdag actief wordt. De klant is tevreden met de informatie en er zijn geen verdere acties nodig.</t>
         </is>
       </c>
-      <c r="F9" t="inlineStr">
+      <c r="H9" t="inlineStr">
         <is>
           <t>bundel informatie</t>
         </is>
       </c>
-      <c r="G9" t="inlineStr">
+      <c r="I9" t="inlineStr">
         <is>
           <t>neutraal</t>
         </is>
       </c>
-      <c r="H9" t="n">
+      <c r="J9" t="n">
         <v>0.00034</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>18491</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="n">
+        <v>8</v>
+      </c>
+      <c r="C10" t="n">
+        <v>18491</v>
+      </c>
+      <c r="D10" t="inlineStr">
         <is>
           <t>2024-09-24 11:03:16</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
+      <c r="E10" t="inlineStr">
         <is>
           <t>Mag u til komen, Henri. Dag hallo met Peter van het Zwarte fietsenplan in Diemen. Hoi. Hoi. Ik krijg de winkel daar niet te pakken en ook even op dit moment niemand op hun mobiel. Kun je zien of de telefonie een probleem heeft, een storing heeft op onze locatie Diemen. Dan kan ik wel even kijken. Ja. Ik zie beide toestellen zie ik offline. Ik krijg geen IP adres terug dus is het internet van Ja, ik weet dat het vaker speelt. Nou vaker is een groot woord, maar het speelt daar af en toe wel dat het netwerk daar niet meer aanwezig is. Oké dat kan je zien in de geschiedenis of zo. Nee, omdat ze wel vaker aan de lijn hebben gelaten dat lui eruit lag. Oké. Ja, ik heb de laatste laatste jaren echt geen geen problemen gehad volgens mij. Nee, op zich valt het wel mee. Ja, het is voornamelijk Roger die in Spanje zit met een schotel die wat problemen ervaart en niemand weet ik gewoon dat er af en toe wat discussie zijn. Maar is ook een tijdje terug weer dus. Ja precies nee ik denk dat dat een tijdje terug is alweer want het gaat nu best wel goed. Ja, klopt inderdaad. Maar ik zie ze nu als zijnde offline en ik krijg ook geen IP-adres terug. Ik kan wel eens monitoring aanzetten. Kijk als ik überhaupt iets terugkijk van een reactie. Wij versturen wel om de zoveel seconden een options pakket om te kijken waar het toestel zich in hun netwerk bevindt om de registratie tot stand te houden. En normaliter reageert het toestel daar wel op, maar aangezien ik nou geen IP-adres terugkrijgt verwacht ik. Nou ik weet niet wat pc nou doet, maar aangezien ik geen IP-adres terugkrijgt verwacht ik dat er in deze netwerk op locatie misschien. Ja precies dat daar iets mee is. Klopt. Goed nou dan Die dacht je iemand met nul zes kunt bereiken. Ja precies heb ik al geprobeerd, maar ik dacht nou als ik ze niet pak uit dan bel ik jullie verrast. Maar goed het lijkt dus geen internet te zijn. Dan ga ik ga ik het opnieuw proberen. Ja, of dat die misschien aangesteld is op het netwerk of dat switchen is uitgevallen. Ik moet die straks trekken dat netwerk er uitlegt, maar normaal die schaal dit wel in die privé terug en dat krijg ik ook niet terug. En als ik nu kijk. De monitoring krijg ik ook geen enkele reactie inderdaad. Nee, oké. Nou ik ga proberen ze te pakken te krijgen. Is goed. Oké bedankt. Oké hoi. Oké, hoi. Alsjeblieft.</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
+      <c r="F10" t="inlineStr">
         <is>
           <t>Peter van het Zwarte Fietsenplan in Diemen belde omdat hij de winkel niet kon bereiken en niemand op hun mobiel kon krijgen. Henri controleerde de situatie en zag dat beide toestellen offline waren en geen IP-adres terugstuurden, wat wijst op een mogelijk netwerkprobleem op de locatie in Diemen. Peter gaat proberen iemand via een mobiel nummer te bereiken en Henri zal monitoring aanzetten om de situatie verder te onderzoeken.</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr">
+      <c r="G10" t="inlineStr">
         <is>
           <t>Peter van het Zwarte fietsenplan belt omdat hij problemen heeft met de telefonie op hun locatie in Diemen. De 10Telecom collega bevestigt dat beide toestellen offline zijn en er geen IP-adres wordt ontvangen. Er wordt gesuggereerd om monitoring aan te zetten om de situatie te controleren. Peter zal proberen contact op te nemen met de winkel om het probleem verder te onderzoeken.</t>
         </is>
       </c>
-      <c r="F10" t="inlineStr">
+      <c r="H10" t="inlineStr">
         <is>
           <t>telefonie storing</t>
         </is>
       </c>
-      <c r="G10" t="inlineStr">
+      <c r="I10" t="inlineStr">
         <is>
           <t>neutraal</t>
         </is>
       </c>
-      <c r="H10" t="n">
+      <c r="J10" t="n">
         <v>0.000441</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>18467</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="n">
+        <v>9</v>
+      </c>
+      <c r="C11" t="n">
+        <v>18467</v>
+      </c>
+      <c r="D11" t="inlineStr">
         <is>
           <t>2024-09-24 09:28:12</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
+      <c r="E11" t="inlineStr">
         <is>
           <t>Nicole, Michael. Michael, megazaak met Jacob. Morgen. Morgen, hoe is het leven? Ja, goede dag, stabiel. Ja, ben je lekker gestart? Ja, zeg maar. Nou, op zich wel, lekker man. Jij ook? Ja, natuurlijk tuurlijk altijd. Alle goed. Als je als je nog een jong kind hebt dan dan start je altijd op tijd op hé. Ja, dan start je altijd goed. Ja, toch? Even een vraagje. Hielk mijn collega die heeft is met Gerel hoveniers bezig geweest. Ja. Alleen die loopt echt wat dingen aan, omdat we natuurlijk wat nieuwere basisstations hebben geleverd. Ja. Ja, nou loopt hij eigenlijk dingen aan dat hij er best wel vaak heen moet. Omdat hij helemaal lekker soepel loopt in die centrale. Heb je iets meegekregen van een w70 mini uit mijn hoofd? Ja, klopt dat is een nieuw systeem van J-Link die kan je dan als zo'n multicel installeren. Ja. Heb jullie enig idee wanneer zo'n profiel geschikt wordt voor autoprovisioning? Normaal gesproken zelf, maar Dat we iets meer op afstand kunnen doen zeg maar. Ja, beetje afhankelijk. Allemaal vrij snel hoor. Nee, oké. Check. Wij moeten er dan wel eentje bestellen dat ik meer op locatie heb om die instellingen dan te checken. Waar loopt die tegenaan? Dingen niet om. Ja. Voor de registratie of? Ja dat soort dingen. Hij kan op basis niet zoveel en nu hebben we die vanochtend gebeld door hem van dat zijn bereik ineens veel minder is geworden 10 opzichte van een vooraf systeem. Maar ja, het lijkt me heel sterk was ook een j-link. Ja, is vaak intern dan toch maar Ja, dus ik ik begrijp dat niet zo heel goed. Het is een term zo'n multicell natuurlijk beter moeten functioneren als een standaard basisstation. Ja, nou want ik zie ook wel dat de registratie is er wel. Ja klopt. Die late zeer vrij laag dus dat zou het probleem niet moeten zijn. Nee nee helder. Nou ik had al gelezen inderdaad over dat systeem dat die dekking wel vrij goed moet zijn. Ja precies en en ja dat roomming schijnt ook niet helemaal lekker te lopen dus ja dus dat zal inderdaad gewoon een intern probleem daar zijn. Ja. Ja, dan zou ik eentje moeten bestellen om daarna te kijken en ook qua bereik. Nee, helder. Dan nog een vraagje. Deze klant die vraagt me ook kan die per extensie ook twee handets koppelen? Mij kan dat niet hoor. Elke handset is een apart extensie. Ja, want dat is een ja, een beperking eigenlijk van het basisstation. Die staat niet toe dat dat twee keer hetzelfde account voorkomt. Nee, check helder. Dus op het moment dat hij bijvoorbeeld zes dus twee per locatie wil laten draaien zou die drie excenties moeten nemen. Klopt, ja. Check is niet zozeer aan ons, want je kan wel twee registratie doen aan onze zijde. Alleen die staat niet toe dat het twee keer hetzelfde kant in komt. Nee, die zegt die bestaat al zeg maar, dat is heel simpel gezegd. Ja. Nee, check helder. Nou ja. Of de andere kom ik even bij terug. Maar dat Ja, dat is helemaal goed. Dat is meer even een vraag van of jullie daar altijd actief mee bezig zijn en en en ik neem aan dat jullie ook de alles erin willen hebben staan natuurlijk. Ja, ja, meestal pakken we dat wel op, ja. Nee, check. Nee, wacht we dat van even af en dan communiceer ik weer met de klant. Ja, oké. Hé, dankjewel jongen. Ja, hoi. Hoi.</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
+      <c r="F11" t="inlineStr">
         <is>
           <t>Nicole belde Michael over problemen met de nieuwe basisstations van J-Link bij Gerel Hoveniers, waar Hielk vaak ter plaatse moet zijn vanwege slecht bereik en registratieproblemen. Michael stelde voor om het nieuwe W70 mini-systeem van J-Link als multicell te installeren en meldde dat autoprovisioning binnenkort beschikbaar zal zijn. Nicole moet een extra unit bestellen om de instellingen en het bereik te controleren. Het koppelen van twee handsets per extensie is niet mogelijk, omdat elke handset een aparte extensie vereist. Nicole zal verdere communicatie met de klant afhandelen.</t>
         </is>
       </c>
-      <c r="E11" t="inlineStr">
+      <c r="G11" t="inlineStr">
         <is>
           <t>Nicole heeft met Michael gesproken over problemen die zijn collega Hielk ondervindt met een nieuw systeem van J-Link. Er is een vraag over de autoprovisioning van een profiel en de dekking van het systeem. Michael bevestigt dat er een intern probleem kan zijn en dat ze een apparaat moeten bestellen om het bereik te controleren. Daarnaast wordt besproken dat een klant niet twee handsets per extensie kan koppelen, wat een beperking van het basisstation is. Michael zal de klant hierover informeren.</t>
         </is>
       </c>
-      <c r="F11" t="inlineStr">
+      <c r="H11" t="inlineStr">
         <is>
           <t>technische ondersteuning</t>
         </is>
       </c>
-      <c r="G11" t="inlineStr">
+      <c r="I11" t="inlineStr">
         <is>
           <t>neutraal</t>
         </is>
       </c>
-      <c r="H11" t="n">
+      <c r="J11" t="n">
         <v>0.000536</v>
       </c>
     </row>

</xml_diff>